<commit_message>
beh piye to kih
</commit_message>
<xml_diff>
--- a/public/excel/import-template.xlsx
+++ b/public/excel/import-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\lansia-care\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECC2D35-215B-4344-B9A8-5EF70EAA9233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DBA849-ACFA-47D7-B10C-3D1B136588EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7CF94693-F0AB-49C7-85BA-72B9B384167A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>NAMALENGKAP</t>
   </si>
@@ -233,6 +233,24 @@
   </si>
   <si>
     <t>RT</t>
+  </si>
+  <si>
+    <t>kognitif</t>
+  </si>
+  <si>
+    <t>mobilisasi</t>
+  </si>
+  <si>
+    <t>depresi</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>malnutrisi</t>
+  </si>
+  <si>
+    <t>Tidak Ada</t>
   </si>
 </sst>
 </file>
@@ -616,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7305E29-93E7-41AD-96E8-BB770E7BFE7B}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,11 +653,15 @@
     <col min="11" max="11" width="15.6640625" style="3" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" style="3" customWidth="1"/>
     <col min="13" max="13" width="14.5546875" style="3" customWidth="1"/>
-    <col min="14" max="27" width="20.88671875" style="3" customWidth="1"/>
-    <col min="28" max="16384" width="8.88671875" style="3"/>
+    <col min="14" max="25" width="20.88671875" style="3" customWidth="1"/>
+    <col min="26" max="32" width="20.77734375" style="3" customWidth="1"/>
+    <col min="33" max="33" width="8.88671875" style="3"/>
+    <col min="34" max="34" width="23.77734375" style="3" customWidth="1"/>
+    <col min="35" max="35" width="21.44140625" style="3" customWidth="1"/>
+    <col min="36" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,14 +737,29 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -798,14 +835,29 @@
       <c r="Y2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -881,14 +933,29 @@
       <c r="Y3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="Z3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
@@ -964,14 +1031,29 @@
       <c r="Y4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="Z4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
@@ -1047,10 +1129,25 @@
       <c r="Y5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>